<commit_message>
revising the lists of hazards and requirements
</commit_message>
<xml_diff>
--- a/org.panorama-research.waters-2019.hazards/waters-challenge-hazards_v2_proposal.xlsx
+++ b/org.panorama-research.waters-2019.hazards/waters-challenge-hazards_v2_proposal.xlsx
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>